<commit_message>
Deploying to gh-pages from @ odomlab2/metadata-submission@8dab341c57736829f8c80f01457da49dbf1c9c79 🚀
</commit_message>
<xml_diff>
--- a/sheets/sequencing_spreadsheet_template.xlsx
+++ b/sheets/sequencing_spreadsheet_template.xlsx
@@ -116,8 +116,8 @@
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Normal" xfId="0" builtinId="0" hidden="0"/>
-    <cellStyle name="-3135089097379038757" xfId="1" hidden="0"/>
-    <cellStyle name="-3343667200349702395" xfId="2" hidden="0"/>
+    <cellStyle name="-1358401275994918282" xfId="1" hidden="0"/>
+    <cellStyle name="2154953909953441353" xfId="2" hidden="0"/>
   </cellStyles>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
   <colors>

</xml_diff>

<commit_message>
Deploying to gh-pages from @ odomlab2/metadata-submission@517f04d038db446e255f9aa13d47de27e935b633 🚀
</commit_message>
<xml_diff>
--- a/sheets/sequencing_spreadsheet_template.xlsx
+++ b/sheets/sequencing_spreadsheet_template.xlsx
@@ -116,8 +116,8 @@
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Normal" xfId="0" builtinId="0" hidden="0"/>
-    <cellStyle name="3901873946584005039" xfId="1" hidden="0"/>
-    <cellStyle name="-2258982165608722130" xfId="2" hidden="0"/>
+    <cellStyle name="4771488770309127727" xfId="1" hidden="0"/>
+    <cellStyle name="3464257487872728269" xfId="2" hidden="0"/>
   </cellStyles>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
   <colors>
@@ -875,7 +875,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:BJ6"/>
+  <dimension ref="A1:BJ7"/>
   <sheetViews>
     <sheetView rightToLeft="0" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
@@ -1328,7 +1328,7 @@
       </c>
       <c r="N2" s="2" t="inlineStr">
         <is>
-          <t>Yes, please!</t>
+          <t>Biological sex of the sampled individual.</t>
         </is>
       </c>
       <c r="O2" s="2" t="inlineStr">
@@ -1795,7 +1795,7 @@
     <row r="4" ht="25" customHeight="1">
       <c r="A4" s="2" t="inlineStr">
         <is>
-          <t>regime</t>
+          <t>used_for</t>
         </is>
       </c>
       <c r="B4" s="2" t="inlineStr">
@@ -1874,26 +1874,106 @@
           <t>Odomlab</t>
         </is>
       </c>
-      <c r="R4" s="2" t="inlineStr"/>
-      <c r="S4" s="2" t="inlineStr"/>
-      <c r="T4" s="2" t="inlineStr"/>
-      <c r="U4" s="2" t="inlineStr"/>
-      <c r="V4" s="2" t="inlineStr"/>
-      <c r="W4" s="2" t="inlineStr"/>
-      <c r="X4" s="2" t="inlineStr"/>
-      <c r="Y4" s="2" t="inlineStr"/>
-      <c r="Z4" s="2" t="inlineStr"/>
-      <c r="AA4" s="2" t="inlineStr"/>
-      <c r="AB4" s="2" t="inlineStr"/>
-      <c r="AC4" s="2" t="inlineStr"/>
-      <c r="AD4" s="2" t="inlineStr"/>
-      <c r="AE4" s="2" t="inlineStr"/>
-      <c r="AF4" s="2" t="inlineStr"/>
-      <c r="AG4" s="2" t="inlineStr"/>
-      <c r="AH4" s="2" t="inlineStr"/>
-      <c r="AI4" s="2" t="inlineStr"/>
-      <c r="AJ4" s="2" t="inlineStr"/>
-      <c r="AK4" s="2" t="inlineStr"/>
+      <c r="R4" s="2" t="inlineStr">
+        <is>
+          <t>Odomlab</t>
+        </is>
+      </c>
+      <c r="S4" s="2" t="inlineStr">
+        <is>
+          <t>Odomlab</t>
+        </is>
+      </c>
+      <c r="T4" s="2" t="inlineStr">
+        <is>
+          <t>Odomlab</t>
+        </is>
+      </c>
+      <c r="U4" s="2" t="inlineStr">
+        <is>
+          <t>Odomlab</t>
+        </is>
+      </c>
+      <c r="V4" s="2" t="inlineStr">
+        <is>
+          <t>Odomlab</t>
+        </is>
+      </c>
+      <c r="W4" s="2" t="inlineStr">
+        <is>
+          <t>Odomlab</t>
+        </is>
+      </c>
+      <c r="X4" s="2" t="inlineStr">
+        <is>
+          <t>Odomlab, GUIDE, OTP</t>
+        </is>
+      </c>
+      <c r="Y4" s="2" t="inlineStr">
+        <is>
+          <t>Odomlab</t>
+        </is>
+      </c>
+      <c r="Z4" s="2" t="inlineStr">
+        <is>
+          <t>Odomlab</t>
+        </is>
+      </c>
+      <c r="AA4" s="2" t="inlineStr">
+        <is>
+          <t>Odomlab</t>
+        </is>
+      </c>
+      <c r="AB4" s="2" t="inlineStr">
+        <is>
+          <t>Odomlab</t>
+        </is>
+      </c>
+      <c r="AC4" s="2" t="inlineStr">
+        <is>
+          <t>Odomlab</t>
+        </is>
+      </c>
+      <c r="AD4" s="2" t="inlineStr">
+        <is>
+          <t>Odomlab</t>
+        </is>
+      </c>
+      <c r="AE4" s="2" t="inlineStr">
+        <is>
+          <t>Odomlab</t>
+        </is>
+      </c>
+      <c r="AF4" s="2" t="inlineStr">
+        <is>
+          <t>Odomlab</t>
+        </is>
+      </c>
+      <c r="AG4" s="2" t="inlineStr">
+        <is>
+          <t>Odomlab</t>
+        </is>
+      </c>
+      <c r="AH4" s="2" t="inlineStr">
+        <is>
+          <t>Odomlab</t>
+        </is>
+      </c>
+      <c r="AI4" s="2" t="inlineStr">
+        <is>
+          <t>Odomlab</t>
+        </is>
+      </c>
+      <c r="AJ4" s="2" t="inlineStr">
+        <is>
+          <t>Odomlab</t>
+        </is>
+      </c>
+      <c r="AK4" s="2" t="inlineStr">
+        <is>
+          <t>Odomlab</t>
+        </is>
+      </c>
       <c r="AL4" s="2" t="inlineStr">
         <is>
           <t>Odomlab</t>
@@ -1924,469 +2004,605 @@
           <t>Odomlab</t>
         </is>
       </c>
-      <c r="AR4" s="2" t="inlineStr"/>
-      <c r="AS4" s="2" t="inlineStr"/>
-      <c r="AT4" s="2" t="inlineStr"/>
-      <c r="AU4" s="2" t="inlineStr"/>
-      <c r="AV4" s="2" t="inlineStr"/>
-      <c r="AW4" s="2" t="inlineStr"/>
-      <c r="AX4" s="2" t="inlineStr"/>
-      <c r="AY4" s="2" t="inlineStr"/>
-      <c r="AZ4" s="2" t="inlineStr"/>
-      <c r="BA4" s="2" t="inlineStr"/>
-      <c r="BB4" s="2" t="inlineStr"/>
+      <c r="AR4" s="2" t="inlineStr">
+        <is>
+          <t>GUIDE, Odomlab</t>
+        </is>
+      </c>
+      <c r="AS4" s="2" t="inlineStr">
+        <is>
+          <t>Odomlab</t>
+        </is>
+      </c>
+      <c r="AT4" s="2" t="inlineStr">
+        <is>
+          <t>Odomlab</t>
+        </is>
+      </c>
+      <c r="AU4" s="2" t="inlineStr">
+        <is>
+          <t>Odomlab</t>
+        </is>
+      </c>
+      <c r="AV4" s="2" t="inlineStr">
+        <is>
+          <t>Odomlab</t>
+        </is>
+      </c>
+      <c r="AW4" s="2" t="inlineStr">
+        <is>
+          <t>Odomlab</t>
+        </is>
+      </c>
+      <c r="AX4" s="2" t="inlineStr">
+        <is>
+          <t>Odomlab</t>
+        </is>
+      </c>
+      <c r="AY4" s="2" t="inlineStr">
+        <is>
+          <t>Odomlab</t>
+        </is>
+      </c>
+      <c r="AZ4" s="2" t="inlineStr">
+        <is>
+          <t>Odomlab</t>
+        </is>
+      </c>
+      <c r="BA4" s="2" t="inlineStr">
+        <is>
+          <t>Odomlab</t>
+        </is>
+      </c>
+      <c r="BB4" s="2" t="inlineStr">
+        <is>
+          <t>Odomlab</t>
+        </is>
+      </c>
       <c r="BC4" s="2" t="inlineStr"/>
-      <c r="BD4" s="2" t="inlineStr"/>
-      <c r="BE4" s="2" t="inlineStr"/>
-      <c r="BF4" s="2" t="inlineStr"/>
-      <c r="BG4" s="2" t="inlineStr"/>
-      <c r="BH4" s="2" t="inlineStr"/>
-      <c r="BI4" s="2" t="inlineStr"/>
-      <c r="BJ4" s="2" t="inlineStr"/>
+      <c r="BD4" s="2" t="inlineStr">
+        <is>
+          <t>Odomlab</t>
+        </is>
+      </c>
+      <c r="BE4" s="2" t="inlineStr">
+        <is>
+          <t>Odomlab</t>
+        </is>
+      </c>
+      <c r="BF4" s="2" t="inlineStr">
+        <is>
+          <t>Odomlab</t>
+        </is>
+      </c>
+      <c r="BG4" s="2" t="inlineStr">
+        <is>
+          <t>Odomlab</t>
+        </is>
+      </c>
+      <c r="BH4" s="2" t="inlineStr">
+        <is>
+          <t>Odomlab</t>
+        </is>
+      </c>
+      <c r="BI4" s="2" t="inlineStr">
+        <is>
+          <t>Odomlab</t>
+        </is>
+      </c>
+      <c r="BJ4" s="2" t="inlineStr">
+        <is>
+          <t>Odomlab</t>
+        </is>
+      </c>
     </row>
     <row r="5" ht="25" customHeight="1">
-      <c r="A5" s="2" t="inlineStr">
-        <is>
-          <t>order</t>
-        </is>
-      </c>
+      <c r="A5" s="2" t="inlineStr"/>
       <c r="B5" s="2" t="inlineStr">
         <is>
           <t>sample</t>
         </is>
       </c>
-      <c r="C5" s="2" t="inlineStr">
-        <is>
-          <t>sample</t>
-        </is>
-      </c>
-      <c r="D5" s="2" t="inlineStr">
-        <is>
-          <t>sample</t>
-        </is>
-      </c>
-      <c r="E5" s="2" t="inlineStr">
-        <is>
-          <t>sample</t>
-        </is>
-      </c>
-      <c r="F5" s="2" t="inlineStr">
-        <is>
-          <t>sample</t>
-        </is>
-      </c>
-      <c r="G5" s="2" t="inlineStr">
-        <is>
-          <t>sample</t>
-        </is>
-      </c>
-      <c r="H5" s="2" t="inlineStr">
-        <is>
-          <t>sample</t>
-        </is>
-      </c>
-      <c r="I5" s="2" t="inlineStr">
-        <is>
-          <t>sample</t>
-        </is>
-      </c>
-      <c r="J5" s="2" t="inlineStr">
-        <is>
-          <t>sample</t>
-        </is>
-      </c>
-      <c r="K5" s="2" t="inlineStr">
-        <is>
-          <t>sample</t>
-        </is>
-      </c>
-      <c r="L5" s="2" t="inlineStr">
-        <is>
-          <t>sample</t>
-        </is>
-      </c>
-      <c r="M5" s="2" t="inlineStr">
-        <is>
-          <t>sample</t>
-        </is>
-      </c>
-      <c r="N5" s="2" t="inlineStr">
-        <is>
-          <t>sample</t>
-        </is>
-      </c>
-      <c r="O5" s="2" t="inlineStr">
-        <is>
-          <t>sample</t>
-        </is>
-      </c>
-      <c r="P5" s="2" t="inlineStr">
-        <is>
-          <t>sample</t>
-        </is>
-      </c>
-      <c r="Q5" s="2" t="inlineStr">
-        <is>
-          <t>sample</t>
-        </is>
-      </c>
-      <c r="R5" s="2" t="inlineStr">
-        <is>
-          <t>sample</t>
-        </is>
-      </c>
-      <c r="S5" s="2" t="inlineStr">
-        <is>
-          <t>experiment</t>
-        </is>
-      </c>
-      <c r="T5" s="2" t="inlineStr">
-        <is>
-          <t>experiment</t>
-        </is>
-      </c>
-      <c r="U5" s="2" t="inlineStr">
-        <is>
-          <t>experiment</t>
-        </is>
-      </c>
-      <c r="V5" s="2" t="inlineStr">
-        <is>
-          <t>experiment</t>
-        </is>
-      </c>
-      <c r="W5" s="2" t="inlineStr">
-        <is>
-          <t>experiment</t>
-        </is>
-      </c>
-      <c r="X5" s="2" t="inlineStr">
-        <is>
-          <t>experiment</t>
-        </is>
-      </c>
-      <c r="Y5" s="2" t="inlineStr">
-        <is>
-          <t>experiment</t>
-        </is>
-      </c>
-      <c r="Z5" s="2" t="inlineStr">
-        <is>
-          <t>experiment</t>
-        </is>
-      </c>
-      <c r="AA5" s="2" t="inlineStr">
-        <is>
-          <t>experiment</t>
-        </is>
-      </c>
-      <c r="AB5" s="2" t="inlineStr">
-        <is>
-          <t>experiment</t>
-        </is>
-      </c>
-      <c r="AC5" s="2" t="inlineStr">
-        <is>
-          <t>experiment</t>
-        </is>
-      </c>
-      <c r="AD5" s="2" t="inlineStr">
-        <is>
-          <t>experiment</t>
-        </is>
-      </c>
-      <c r="AE5" s="2" t="inlineStr">
-        <is>
-          <t>experiment</t>
-        </is>
-      </c>
-      <c r="AF5" s="2" t="inlineStr">
-        <is>
-          <t>experiment</t>
-        </is>
-      </c>
-      <c r="AG5" s="2" t="inlineStr">
-        <is>
-          <t>experiment</t>
-        </is>
-      </c>
-      <c r="AH5" s="2" t="inlineStr">
-        <is>
-          <t>experiment</t>
-        </is>
-      </c>
-      <c r="AI5" s="2" t="inlineStr">
-        <is>
-          <t>experiment</t>
-        </is>
-      </c>
-      <c r="AJ5" s="2" t="inlineStr">
-        <is>
-          <t>experiment</t>
-        </is>
-      </c>
-      <c r="AK5" s="2" t="inlineStr">
-        <is>
-          <t>experiment</t>
-        </is>
-      </c>
-      <c r="AL5" s="2" t="inlineStr">
-        <is>
-          <t>experiment</t>
-        </is>
-      </c>
-      <c r="AM5" s="2" t="inlineStr">
-        <is>
-          <t>experiment</t>
-        </is>
-      </c>
-      <c r="AN5" s="2" t="inlineStr">
-        <is>
-          <t>sequencing</t>
-        </is>
-      </c>
-      <c r="AO5" s="2" t="inlineStr">
-        <is>
-          <t>sequencing</t>
-        </is>
-      </c>
-      <c r="AP5" s="2" t="inlineStr">
-        <is>
-          <t>sequencing</t>
-        </is>
-      </c>
-      <c r="AQ5" s="2" t="inlineStr">
-        <is>
-          <t>sequencing</t>
-        </is>
-      </c>
-      <c r="AR5" s="2" t="inlineStr">
-        <is>
-          <t>sequencing</t>
-        </is>
-      </c>
-      <c r="AS5" s="2" t="inlineStr">
-        <is>
-          <t>sequencing</t>
-        </is>
-      </c>
-      <c r="AT5" s="2" t="inlineStr">
-        <is>
-          <t>sequencing</t>
-        </is>
-      </c>
-      <c r="AU5" s="2" t="inlineStr">
-        <is>
-          <t>sequencing</t>
-        </is>
-      </c>
-      <c r="AV5" s="2" t="inlineStr">
-        <is>
-          <t>sequencing</t>
-        </is>
-      </c>
-      <c r="AW5" s="2" t="inlineStr">
-        <is>
-          <t>sequencing</t>
-        </is>
-      </c>
-      <c r="AX5" s="2" t="inlineStr">
-        <is>
-          <t>sequencing</t>
-        </is>
-      </c>
-      <c r="AY5" s="2" t="inlineStr">
-        <is>
-          <t>other</t>
-        </is>
-      </c>
-      <c r="AZ5" s="2" t="inlineStr">
-        <is>
-          <t>other</t>
-        </is>
-      </c>
-      <c r="BA5" s="2" t="inlineStr">
-        <is>
-          <t>other</t>
-        </is>
-      </c>
-      <c r="BB5" s="2" t="inlineStr">
-        <is>
-          <t>other</t>
-        </is>
-      </c>
-      <c r="BC5" s="2" t="inlineStr">
-        <is>
-          <t>other</t>
-        </is>
-      </c>
-      <c r="BD5" s="2" t="inlineStr">
-        <is>
-          <t>other</t>
-        </is>
-      </c>
-      <c r="BE5" s="2" t="inlineStr">
-        <is>
-          <t>other</t>
-        </is>
-      </c>
-      <c r="BF5" s="2" t="inlineStr">
-        <is>
-          <t>other</t>
-        </is>
-      </c>
-      <c r="BG5" s="2" t="inlineStr">
-        <is>
-          <t>other</t>
-        </is>
-      </c>
-      <c r="BH5" s="2" t="inlineStr">
-        <is>
-          <t>other</t>
-        </is>
-      </c>
-      <c r="BI5" s="2" t="inlineStr">
-        <is>
-          <t>other</t>
-        </is>
-      </c>
-      <c r="BJ5" s="2" t="inlineStr">
-        <is>
-          <t>other</t>
-        </is>
-      </c>
+      <c r="C5" s="2" t="inlineStr"/>
+      <c r="D5" s="2" t="inlineStr"/>
+      <c r="E5" s="2" t="inlineStr"/>
+      <c r="F5" s="2" t="inlineStr"/>
+      <c r="G5" s="2" t="inlineStr"/>
+      <c r="H5" s="2" t="inlineStr"/>
+      <c r="I5" s="2" t="inlineStr"/>
+      <c r="J5" s="2" t="inlineStr"/>
+      <c r="K5" s="2" t="inlineStr"/>
+      <c r="L5" s="2" t="inlineStr"/>
+      <c r="M5" s="2" t="inlineStr"/>
+      <c r="N5" s="2" t="inlineStr"/>
+      <c r="O5" s="2" t="inlineStr"/>
+      <c r="P5" s="2" t="inlineStr"/>
+      <c r="Q5" s="2" t="inlineStr"/>
+      <c r="R5" s="2" t="inlineStr"/>
+      <c r="S5" s="2" t="inlineStr"/>
+      <c r="T5" s="2" t="inlineStr"/>
+      <c r="U5" s="2" t="inlineStr"/>
+      <c r="V5" s="2" t="inlineStr"/>
+      <c r="W5" s="2" t="inlineStr"/>
+      <c r="X5" s="2" t="inlineStr"/>
+      <c r="Y5" s="2" t="inlineStr"/>
+      <c r="Z5" s="2" t="inlineStr"/>
+      <c r="AA5" s="2" t="inlineStr"/>
+      <c r="AB5" s="2" t="inlineStr"/>
+      <c r="AC5" s="2" t="inlineStr"/>
+      <c r="AD5" s="2" t="inlineStr"/>
+      <c r="AE5" s="2" t="inlineStr"/>
+      <c r="AF5" s="2" t="inlineStr"/>
+      <c r="AG5" s="2" t="inlineStr"/>
+      <c r="AH5" s="2" t="inlineStr"/>
+      <c r="AI5" s="2" t="inlineStr"/>
+      <c r="AJ5" s="2" t="inlineStr"/>
+      <c r="AK5" s="2" t="inlineStr"/>
+      <c r="AL5" s="2" t="inlineStr"/>
+      <c r="AM5" s="2" t="inlineStr"/>
+      <c r="AN5" s="2" t="inlineStr"/>
+      <c r="AO5" s="2" t="inlineStr"/>
+      <c r="AP5" s="2" t="inlineStr"/>
+      <c r="AQ5" s="2" t="inlineStr"/>
+      <c r="AR5" s="2" t="inlineStr"/>
+      <c r="AS5" s="2" t="inlineStr"/>
+      <c r="AT5" s="2" t="inlineStr"/>
+      <c r="AU5" s="2" t="inlineStr"/>
+      <c r="AV5" s="2" t="inlineStr"/>
+      <c r="AW5" s="2" t="inlineStr"/>
+      <c r="AX5" s="2" t="inlineStr"/>
+      <c r="AY5" s="2" t="inlineStr"/>
+      <c r="AZ5" s="2" t="inlineStr"/>
+      <c r="BA5" s="2" t="inlineStr"/>
+      <c r="BB5" s="2" t="inlineStr"/>
+      <c r="BC5" s="2" t="inlineStr"/>
+      <c r="BD5" s="2" t="inlineStr"/>
+      <c r="BE5" s="2" t="inlineStr"/>
+      <c r="BF5" s="2" t="inlineStr"/>
+      <c r="BG5" s="2" t="inlineStr"/>
+      <c r="BH5" s="2" t="inlineStr"/>
+      <c r="BI5" s="2" t="inlineStr"/>
+      <c r="BJ5" s="2" t="inlineStr"/>
     </row>
     <row r="6" ht="25" customHeight="1">
       <c r="A6" s="2" t="inlineStr">
         <is>
+          <t>category</t>
+        </is>
+      </c>
+      <c r="B6" s="2" t="inlineStr"/>
+      <c r="C6" s="2" t="inlineStr">
+        <is>
+          <t>sample</t>
+        </is>
+      </c>
+      <c r="D6" s="2" t="inlineStr">
+        <is>
+          <t>sample</t>
+        </is>
+      </c>
+      <c r="E6" s="2" t="inlineStr">
+        <is>
+          <t>sample</t>
+        </is>
+      </c>
+      <c r="F6" s="2" t="inlineStr">
+        <is>
+          <t>sample</t>
+        </is>
+      </c>
+      <c r="G6" s="2" t="inlineStr">
+        <is>
+          <t>sample</t>
+        </is>
+      </c>
+      <c r="H6" s="2" t="inlineStr">
+        <is>
+          <t>sample</t>
+        </is>
+      </c>
+      <c r="I6" s="2" t="inlineStr">
+        <is>
+          <t>sample</t>
+        </is>
+      </c>
+      <c r="J6" s="2" t="inlineStr">
+        <is>
+          <t>sample</t>
+        </is>
+      </c>
+      <c r="K6" s="2" t="inlineStr">
+        <is>
+          <t>sample</t>
+        </is>
+      </c>
+      <c r="L6" s="2" t="inlineStr">
+        <is>
+          <t>sample</t>
+        </is>
+      </c>
+      <c r="M6" s="2" t="inlineStr">
+        <is>
+          <t>sample</t>
+        </is>
+      </c>
+      <c r="N6" s="2" t="inlineStr">
+        <is>
+          <t>sample</t>
+        </is>
+      </c>
+      <c r="O6" s="2" t="inlineStr">
+        <is>
+          <t>sample</t>
+        </is>
+      </c>
+      <c r="P6" s="2" t="inlineStr">
+        <is>
+          <t>sample</t>
+        </is>
+      </c>
+      <c r="Q6" s="2" t="inlineStr">
+        <is>
+          <t>sample</t>
+        </is>
+      </c>
+      <c r="R6" s="2" t="inlineStr">
+        <is>
+          <t>sample</t>
+        </is>
+      </c>
+      <c r="S6" s="2" t="inlineStr">
+        <is>
+          <t>experiment</t>
+        </is>
+      </c>
+      <c r="T6" s="2" t="inlineStr">
+        <is>
+          <t>experiment</t>
+        </is>
+      </c>
+      <c r="U6" s="2" t="inlineStr">
+        <is>
+          <t>experiment</t>
+        </is>
+      </c>
+      <c r="V6" s="2" t="inlineStr">
+        <is>
+          <t>experiment</t>
+        </is>
+      </c>
+      <c r="W6" s="2" t="inlineStr">
+        <is>
+          <t>experiment</t>
+        </is>
+      </c>
+      <c r="X6" s="2" t="inlineStr">
+        <is>
+          <t>experiment</t>
+        </is>
+      </c>
+      <c r="Y6" s="2" t="inlineStr">
+        <is>
+          <t>experiment</t>
+        </is>
+      </c>
+      <c r="Z6" s="2" t="inlineStr">
+        <is>
+          <t>experiment</t>
+        </is>
+      </c>
+      <c r="AA6" s="2" t="inlineStr">
+        <is>
+          <t>experiment</t>
+        </is>
+      </c>
+      <c r="AB6" s="2" t="inlineStr">
+        <is>
+          <t>experiment</t>
+        </is>
+      </c>
+      <c r="AC6" s="2" t="inlineStr">
+        <is>
+          <t>experiment</t>
+        </is>
+      </c>
+      <c r="AD6" s="2" t="inlineStr">
+        <is>
+          <t>experiment</t>
+        </is>
+      </c>
+      <c r="AE6" s="2" t="inlineStr">
+        <is>
+          <t>experiment</t>
+        </is>
+      </c>
+      <c r="AF6" s="2" t="inlineStr">
+        <is>
+          <t>experiment</t>
+        </is>
+      </c>
+      <c r="AG6" s="2" t="inlineStr">
+        <is>
+          <t>experiment</t>
+        </is>
+      </c>
+      <c r="AH6" s="2" t="inlineStr">
+        <is>
+          <t>experiment</t>
+        </is>
+      </c>
+      <c r="AI6" s="2" t="inlineStr">
+        <is>
+          <t>experiment</t>
+        </is>
+      </c>
+      <c r="AJ6" s="2" t="inlineStr">
+        <is>
+          <t>experiment</t>
+        </is>
+      </c>
+      <c r="AK6" s="2" t="inlineStr">
+        <is>
+          <t>experiment</t>
+        </is>
+      </c>
+      <c r="AL6" s="2" t="inlineStr">
+        <is>
+          <t>experiment</t>
+        </is>
+      </c>
+      <c r="AM6" s="2" t="inlineStr">
+        <is>
+          <t>experiment</t>
+        </is>
+      </c>
+      <c r="AN6" s="2" t="inlineStr">
+        <is>
+          <t>sequencing</t>
+        </is>
+      </c>
+      <c r="AO6" s="2" t="inlineStr">
+        <is>
+          <t>sequencing</t>
+        </is>
+      </c>
+      <c r="AP6" s="2" t="inlineStr">
+        <is>
+          <t>sequencing</t>
+        </is>
+      </c>
+      <c r="AQ6" s="2" t="inlineStr">
+        <is>
+          <t>sequencing</t>
+        </is>
+      </c>
+      <c r="AR6" s="2" t="inlineStr">
+        <is>
+          <t>sequencing</t>
+        </is>
+      </c>
+      <c r="AS6" s="2" t="inlineStr">
+        <is>
+          <t>sequencing</t>
+        </is>
+      </c>
+      <c r="AT6" s="2" t="inlineStr">
+        <is>
+          <t>sequencing</t>
+        </is>
+      </c>
+      <c r="AU6" s="2" t="inlineStr">
+        <is>
+          <t>sequencing</t>
+        </is>
+      </c>
+      <c r="AV6" s="2" t="inlineStr">
+        <is>
+          <t>sequencing</t>
+        </is>
+      </c>
+      <c r="AW6" s="2" t="inlineStr">
+        <is>
+          <t>sequencing</t>
+        </is>
+      </c>
+      <c r="AX6" s="2" t="inlineStr">
+        <is>
+          <t>sequencing</t>
+        </is>
+      </c>
+      <c r="AY6" s="2" t="inlineStr">
+        <is>
+          <t>other</t>
+        </is>
+      </c>
+      <c r="AZ6" s="2" t="inlineStr">
+        <is>
+          <t>other</t>
+        </is>
+      </c>
+      <c r="BA6" s="2" t="inlineStr">
+        <is>
+          <t>other</t>
+        </is>
+      </c>
+      <c r="BB6" s="2" t="inlineStr">
+        <is>
+          <t>other</t>
+        </is>
+      </c>
+      <c r="BC6" s="2" t="inlineStr">
+        <is>
+          <t>other</t>
+        </is>
+      </c>
+      <c r="BD6" s="2" t="inlineStr">
+        <is>
+          <t>other</t>
+        </is>
+      </c>
+      <c r="BE6" s="2" t="inlineStr">
+        <is>
+          <t>other</t>
+        </is>
+      </c>
+      <c r="BF6" s="2" t="inlineStr">
+        <is>
+          <t>other</t>
+        </is>
+      </c>
+      <c r="BG6" s="2" t="inlineStr">
+        <is>
+          <t>other</t>
+        </is>
+      </c>
+      <c r="BH6" s="2" t="inlineStr">
+        <is>
+          <t>other</t>
+        </is>
+      </c>
+      <c r="BI6" s="2" t="inlineStr">
+        <is>
+          <t>other</t>
+        </is>
+      </c>
+      <c r="BJ6" s="2" t="inlineStr">
+        <is>
+          <t>other</t>
+        </is>
+      </c>
+    </row>
+    <row r="7" ht="25" customHeight="1">
+      <c r="A7" s="2" t="inlineStr">
+        <is>
           <t>regex</t>
         </is>
       </c>
-      <c r="B6" s="2" t="inlineStr"/>
-      <c r="C6" s="2" t="inlineStr"/>
-      <c r="D6" s="2" t="inlineStr"/>
-      <c r="E6" s="2" t="inlineStr"/>
-      <c r="F6" s="2" t="inlineStr"/>
-      <c r="G6" s="2" t="inlineStr"/>
-      <c r="H6" s="2" t="inlineStr"/>
-      <c r="I6" s="2" t="inlineStr"/>
-      <c r="J6" s="2" t="inlineStr"/>
-      <c r="K6" s="2" t="inlineStr"/>
-      <c r="L6" s="2" t="inlineStr"/>
-      <c r="M6" s="2" t="inlineStr"/>
-      <c r="N6" s="2" t="inlineStr"/>
-      <c r="O6" s="2" t="inlineStr"/>
-      <c r="P6" s="2" t="inlineStr"/>
-      <c r="Q6" s="2" t="inlineStr"/>
-      <c r="R6" s="2" t="inlineStr"/>
-      <c r="S6" s="2" t="inlineStr"/>
-      <c r="T6" s="2" t="inlineStr"/>
-      <c r="U6" s="2" t="inlineStr"/>
-      <c r="V6" s="2" t="inlineStr"/>
-      <c r="W6" s="2" t="inlineStr"/>
-      <c r="X6" s="2" t="inlineStr"/>
-      <c r="Y6" s="2" t="inlineStr"/>
-      <c r="Z6" s="2" t="inlineStr">
+      <c r="B7" s="2" t="inlineStr"/>
+      <c r="C7" s="2" t="inlineStr"/>
+      <c r="D7" s="2" t="inlineStr"/>
+      <c r="E7" s="2" t="inlineStr"/>
+      <c r="F7" s="2" t="inlineStr"/>
+      <c r="G7" s="2" t="inlineStr"/>
+      <c r="H7" s="2" t="inlineStr"/>
+      <c r="I7" s="2" t="inlineStr"/>
+      <c r="J7" s="2" t="inlineStr"/>
+      <c r="K7" s="2" t="inlineStr"/>
+      <c r="L7" s="2" t="inlineStr"/>
+      <c r="M7" s="2" t="inlineStr"/>
+      <c r="N7" s="2" t="inlineStr"/>
+      <c r="O7" s="2" t="inlineStr"/>
+      <c r="P7" s="2" t="inlineStr"/>
+      <c r="Q7" s="2" t="inlineStr"/>
+      <c r="R7" s="2" t="inlineStr"/>
+      <c r="S7" s="2" t="inlineStr"/>
+      <c r="T7" s="2" t="inlineStr"/>
+      <c r="U7" s="2" t="inlineStr"/>
+      <c r="V7" s="2" t="inlineStr"/>
+      <c r="W7" s="2" t="inlineStr"/>
+      <c r="X7" s="2" t="inlineStr"/>
+      <c r="Y7" s="2" t="inlineStr"/>
+      <c r="Z7" s="2" t="inlineStr">
         <is>
           <t>[+-]?([0-9]*[.])?[0-9]+</t>
         </is>
       </c>
-      <c r="AA6" s="2" t="inlineStr">
+      <c r="AA7" s="2" t="inlineStr">
         <is>
           <t>[+-]?([0-9]*[.])?[0-9]+</t>
         </is>
       </c>
-      <c r="AB6" s="2" t="inlineStr">
+      <c r="AB7" s="2" t="inlineStr">
         <is>
           <t>[0-9]*</t>
         </is>
       </c>
-      <c r="AC6" s="2" t="inlineStr">
+      <c r="AC7" s="2" t="inlineStr">
         <is>
           <t>[0-9]*</t>
         </is>
       </c>
-      <c r="AD6" s="2" t="inlineStr">
+      <c r="AD7" s="2" t="inlineStr">
         <is>
           <t>[+-]?([0-9]*[.])?[0-9]+</t>
         </is>
       </c>
-      <c r="AE6" s="2" t="inlineStr">
+      <c r="AE7" s="2" t="inlineStr">
         <is>
           <t>[0-9]*</t>
         </is>
       </c>
-      <c r="AF6" s="2" t="inlineStr">
+      <c r="AF7" s="2" t="inlineStr">
         <is>
           <t>[+-]?([0-9]*[.])?[0-9]+</t>
         </is>
       </c>
-      <c r="AG6" s="2" t="inlineStr"/>
-      <c r="AH6" s="2" t="inlineStr"/>
-      <c r="AI6" s="2" t="inlineStr">
+      <c r="AG7" s="2" t="inlineStr"/>
+      <c r="AH7" s="2" t="inlineStr"/>
+      <c r="AI7" s="2" t="inlineStr">
         <is>
           <t>[ATGC]*</t>
         </is>
       </c>
-      <c r="AJ6" s="2" t="inlineStr"/>
-      <c r="AK6" s="2" t="inlineStr">
+      <c r="AJ7" s="2" t="inlineStr"/>
+      <c r="AK7" s="2" t="inlineStr">
         <is>
           <t>[ATGC, ]*</t>
         </is>
       </c>
-      <c r="AL6" s="2" t="inlineStr"/>
-      <c r="AM6" s="2" t="inlineStr"/>
-      <c r="AN6" s="2" t="inlineStr"/>
-      <c r="AO6" s="2" t="inlineStr">
+      <c r="AL7" s="2" t="inlineStr"/>
+      <c r="AM7" s="2" t="inlineStr"/>
+      <c r="AN7" s="2" t="inlineStr"/>
+      <c r="AO7" s="2" t="inlineStr">
         <is>
           <t>[0-9]*</t>
         </is>
       </c>
-      <c r="AP6" s="2" t="inlineStr">
+      <c r="AP7" s="2" t="inlineStr">
         <is>
           <t>[A-Z]{2}[0-9]{4}[0-9]{2}[0-9]{2}</t>
         </is>
       </c>
-      <c r="AQ6" s="2" t="inlineStr">
+      <c r="AQ7" s="2" t="inlineStr">
         <is>
           <t>[0-9]*</t>
         </is>
       </c>
-      <c r="AR6" s="2" t="inlineStr">
+      <c r="AR7" s="2" t="inlineStr">
         <is>
           <t>[0-9]{5,}</t>
         </is>
       </c>
-      <c r="AS6" s="2" t="inlineStr"/>
-      <c r="AT6" s="2" t="inlineStr"/>
-      <c r="AU6" s="2" t="inlineStr"/>
-      <c r="AV6" s="2" t="inlineStr">
+      <c r="AS7" s="2" t="inlineStr"/>
+      <c r="AT7" s="2" t="inlineStr"/>
+      <c r="AU7" s="2" t="inlineStr"/>
+      <c r="AV7" s="2" t="inlineStr">
         <is>
           <t>[0-9]{1,2}</t>
         </is>
       </c>
-      <c r="AW6" s="2" t="inlineStr">
+      <c r="AW7" s="2" t="inlineStr">
         <is>
           <t>[A-Z]</t>
         </is>
       </c>
-      <c r="AX6" s="2" t="inlineStr">
+      <c r="AX7" s="2" t="inlineStr">
         <is>
           <t>[0-9]{1,2}[A-Z]</t>
         </is>
       </c>
-      <c r="AY6" s="2" t="inlineStr"/>
-      <c r="AZ6" s="2" t="inlineStr"/>
-      <c r="BA6" s="2" t="inlineStr"/>
-      <c r="BB6" s="2" t="inlineStr"/>
-      <c r="BC6" s="2" t="inlineStr"/>
-      <c r="BD6" s="2" t="inlineStr"/>
-      <c r="BE6" s="2" t="inlineStr"/>
-      <c r="BF6" s="2" t="inlineStr"/>
-      <c r="BG6" s="2" t="inlineStr"/>
-      <c r="BH6" s="2" t="inlineStr"/>
-      <c r="BI6" s="2" t="inlineStr"/>
-      <c r="BJ6" s="2" t="inlineStr"/>
+      <c r="AY7" s="2" t="inlineStr"/>
+      <c r="AZ7" s="2" t="inlineStr"/>
+      <c r="BA7" s="2" t="inlineStr"/>
+      <c r="BB7" s="2" t="inlineStr"/>
+      <c r="BC7" s="2" t="inlineStr"/>
+      <c r="BD7" s="2" t="inlineStr"/>
+      <c r="BE7" s="2" t="inlineStr"/>
+      <c r="BF7" s="2" t="inlineStr"/>
+      <c r="BG7" s="2" t="inlineStr"/>
+      <c r="BH7" s="2" t="inlineStr"/>
+      <c r="BI7" s="2" t="inlineStr"/>
+      <c r="BJ7" s="2" t="inlineStr"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>

<commit_message>
Deploying to gh-pages from @ odomlab2/metadata-submission@80c35e5bec056d1c37b492ac345ebcf4c9da9408 🚀
</commit_message>
<xml_diff>
--- a/sheets/sequencing_spreadsheet_template.xlsx
+++ b/sheets/sequencing_spreadsheet_template.xlsx
@@ -116,8 +116,8 @@
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Normal" xfId="0" builtinId="0" hidden="0"/>
-    <cellStyle name="4771488770309127727" xfId="1" hidden="0"/>
-    <cellStyle name="3464257487872728269" xfId="2" hidden="0"/>
+    <cellStyle name="-8821748414531298053" xfId="1" hidden="0"/>
+    <cellStyle name="6220453436343325599" xfId="2" hidden="0"/>
   </cellStyles>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
   <colors>
@@ -875,7 +875,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:BJ7"/>
+  <dimension ref="A1:BJ6"/>
   <sheetViews>
     <sheetView rightToLeft="0" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
@@ -2097,512 +2097,448 @@
       </c>
     </row>
     <row r="5" ht="25" customHeight="1">
-      <c r="A5" s="2" t="inlineStr"/>
+      <c r="A5" s="2" t="inlineStr">
+        <is>
+          <t>category</t>
+        </is>
+      </c>
       <c r="B5" s="2" t="inlineStr">
         <is>
           <t>sample</t>
         </is>
       </c>
-      <c r="C5" s="2" t="inlineStr"/>
-      <c r="D5" s="2" t="inlineStr"/>
-      <c r="E5" s="2" t="inlineStr"/>
-      <c r="F5" s="2" t="inlineStr"/>
-      <c r="G5" s="2" t="inlineStr"/>
-      <c r="H5" s="2" t="inlineStr"/>
-      <c r="I5" s="2" t="inlineStr"/>
-      <c r="J5" s="2" t="inlineStr"/>
-      <c r="K5" s="2" t="inlineStr"/>
-      <c r="L5" s="2" t="inlineStr"/>
-      <c r="M5" s="2" t="inlineStr"/>
-      <c r="N5" s="2" t="inlineStr"/>
-      <c r="O5" s="2" t="inlineStr"/>
-      <c r="P5" s="2" t="inlineStr"/>
-      <c r="Q5" s="2" t="inlineStr"/>
-      <c r="R5" s="2" t="inlineStr"/>
-      <c r="S5" s="2" t="inlineStr"/>
-      <c r="T5" s="2" t="inlineStr"/>
-      <c r="U5" s="2" t="inlineStr"/>
-      <c r="V5" s="2" t="inlineStr"/>
-      <c r="W5" s="2" t="inlineStr"/>
-      <c r="X5" s="2" t="inlineStr"/>
-      <c r="Y5" s="2" t="inlineStr"/>
-      <c r="Z5" s="2" t="inlineStr"/>
-      <c r="AA5" s="2" t="inlineStr"/>
-      <c r="AB5" s="2" t="inlineStr"/>
-      <c r="AC5" s="2" t="inlineStr"/>
-      <c r="AD5" s="2" t="inlineStr"/>
-      <c r="AE5" s="2" t="inlineStr"/>
-      <c r="AF5" s="2" t="inlineStr"/>
-      <c r="AG5" s="2" t="inlineStr"/>
-      <c r="AH5" s="2" t="inlineStr"/>
-      <c r="AI5" s="2" t="inlineStr"/>
-      <c r="AJ5" s="2" t="inlineStr"/>
-      <c r="AK5" s="2" t="inlineStr"/>
-      <c r="AL5" s="2" t="inlineStr"/>
-      <c r="AM5" s="2" t="inlineStr"/>
-      <c r="AN5" s="2" t="inlineStr"/>
-      <c r="AO5" s="2" t="inlineStr"/>
-      <c r="AP5" s="2" t="inlineStr"/>
-      <c r="AQ5" s="2" t="inlineStr"/>
-      <c r="AR5" s="2" t="inlineStr"/>
-      <c r="AS5" s="2" t="inlineStr"/>
-      <c r="AT5" s="2" t="inlineStr"/>
-      <c r="AU5" s="2" t="inlineStr"/>
-      <c r="AV5" s="2" t="inlineStr"/>
-      <c r="AW5" s="2" t="inlineStr"/>
-      <c r="AX5" s="2" t="inlineStr"/>
-      <c r="AY5" s="2" t="inlineStr"/>
-      <c r="AZ5" s="2" t="inlineStr"/>
-      <c r="BA5" s="2" t="inlineStr"/>
-      <c r="BB5" s="2" t="inlineStr"/>
-      <c r="BC5" s="2" t="inlineStr"/>
-      <c r="BD5" s="2" t="inlineStr"/>
-      <c r="BE5" s="2" t="inlineStr"/>
-      <c r="BF5" s="2" t="inlineStr"/>
-      <c r="BG5" s="2" t="inlineStr"/>
-      <c r="BH5" s="2" t="inlineStr"/>
-      <c r="BI5" s="2" t="inlineStr"/>
-      <c r="BJ5" s="2" t="inlineStr"/>
+      <c r="C5" s="2" t="inlineStr">
+        <is>
+          <t>sample</t>
+        </is>
+      </c>
+      <c r="D5" s="2" t="inlineStr">
+        <is>
+          <t>sample</t>
+        </is>
+      </c>
+      <c r="E5" s="2" t="inlineStr">
+        <is>
+          <t>sample</t>
+        </is>
+      </c>
+      <c r="F5" s="2" t="inlineStr">
+        <is>
+          <t>sample</t>
+        </is>
+      </c>
+      <c r="G5" s="2" t="inlineStr">
+        <is>
+          <t>sample</t>
+        </is>
+      </c>
+      <c r="H5" s="2" t="inlineStr">
+        <is>
+          <t>sample</t>
+        </is>
+      </c>
+      <c r="I5" s="2" t="inlineStr">
+        <is>
+          <t>sample</t>
+        </is>
+      </c>
+      <c r="J5" s="2" t="inlineStr">
+        <is>
+          <t>sample</t>
+        </is>
+      </c>
+      <c r="K5" s="2" t="inlineStr">
+        <is>
+          <t>sample</t>
+        </is>
+      </c>
+      <c r="L5" s="2" t="inlineStr">
+        <is>
+          <t>sample</t>
+        </is>
+      </c>
+      <c r="M5" s="2" t="inlineStr">
+        <is>
+          <t>sample</t>
+        </is>
+      </c>
+      <c r="N5" s="2" t="inlineStr">
+        <is>
+          <t>sample</t>
+        </is>
+      </c>
+      <c r="O5" s="2" t="inlineStr">
+        <is>
+          <t>sample</t>
+        </is>
+      </c>
+      <c r="P5" s="2" t="inlineStr">
+        <is>
+          <t>sample</t>
+        </is>
+      </c>
+      <c r="Q5" s="2" t="inlineStr">
+        <is>
+          <t>sample</t>
+        </is>
+      </c>
+      <c r="R5" s="2" t="inlineStr">
+        <is>
+          <t>sample</t>
+        </is>
+      </c>
+      <c r="S5" s="2" t="inlineStr">
+        <is>
+          <t>experiment</t>
+        </is>
+      </c>
+      <c r="T5" s="2" t="inlineStr">
+        <is>
+          <t>experiment</t>
+        </is>
+      </c>
+      <c r="U5" s="2" t="inlineStr">
+        <is>
+          <t>experiment</t>
+        </is>
+      </c>
+      <c r="V5" s="2" t="inlineStr">
+        <is>
+          <t>experiment</t>
+        </is>
+      </c>
+      <c r="W5" s="2" t="inlineStr">
+        <is>
+          <t>experiment</t>
+        </is>
+      </c>
+      <c r="X5" s="2" t="inlineStr">
+        <is>
+          <t>experiment</t>
+        </is>
+      </c>
+      <c r="Y5" s="2" t="inlineStr">
+        <is>
+          <t>experiment</t>
+        </is>
+      </c>
+      <c r="Z5" s="2" t="inlineStr">
+        <is>
+          <t>experiment</t>
+        </is>
+      </c>
+      <c r="AA5" s="2" t="inlineStr">
+        <is>
+          <t>experiment</t>
+        </is>
+      </c>
+      <c r="AB5" s="2" t="inlineStr">
+        <is>
+          <t>experiment</t>
+        </is>
+      </c>
+      <c r="AC5" s="2" t="inlineStr">
+        <is>
+          <t>experiment</t>
+        </is>
+      </c>
+      <c r="AD5" s="2" t="inlineStr">
+        <is>
+          <t>experiment</t>
+        </is>
+      </c>
+      <c r="AE5" s="2" t="inlineStr">
+        <is>
+          <t>experiment</t>
+        </is>
+      </c>
+      <c r="AF5" s="2" t="inlineStr">
+        <is>
+          <t>experiment</t>
+        </is>
+      </c>
+      <c r="AG5" s="2" t="inlineStr">
+        <is>
+          <t>experiment</t>
+        </is>
+      </c>
+      <c r="AH5" s="2" t="inlineStr">
+        <is>
+          <t>experiment</t>
+        </is>
+      </c>
+      <c r="AI5" s="2" t="inlineStr">
+        <is>
+          <t>experiment</t>
+        </is>
+      </c>
+      <c r="AJ5" s="2" t="inlineStr">
+        <is>
+          <t>experiment</t>
+        </is>
+      </c>
+      <c r="AK5" s="2" t="inlineStr">
+        <is>
+          <t>experiment</t>
+        </is>
+      </c>
+      <c r="AL5" s="2" t="inlineStr">
+        <is>
+          <t>experiment</t>
+        </is>
+      </c>
+      <c r="AM5" s="2" t="inlineStr">
+        <is>
+          <t>experiment</t>
+        </is>
+      </c>
+      <c r="AN5" s="2" t="inlineStr">
+        <is>
+          <t>sequencing</t>
+        </is>
+      </c>
+      <c r="AO5" s="2" t="inlineStr">
+        <is>
+          <t>sequencing</t>
+        </is>
+      </c>
+      <c r="AP5" s="2" t="inlineStr">
+        <is>
+          <t>sequencing</t>
+        </is>
+      </c>
+      <c r="AQ5" s="2" t="inlineStr">
+        <is>
+          <t>sequencing</t>
+        </is>
+      </c>
+      <c r="AR5" s="2" t="inlineStr">
+        <is>
+          <t>sequencing</t>
+        </is>
+      </c>
+      <c r="AS5" s="2" t="inlineStr">
+        <is>
+          <t>sequencing</t>
+        </is>
+      </c>
+      <c r="AT5" s="2" t="inlineStr">
+        <is>
+          <t>sequencing</t>
+        </is>
+      </c>
+      <c r="AU5" s="2" t="inlineStr">
+        <is>
+          <t>sequencing</t>
+        </is>
+      </c>
+      <c r="AV5" s="2" t="inlineStr">
+        <is>
+          <t>sequencing</t>
+        </is>
+      </c>
+      <c r="AW5" s="2" t="inlineStr">
+        <is>
+          <t>sequencing</t>
+        </is>
+      </c>
+      <c r="AX5" s="2" t="inlineStr">
+        <is>
+          <t>sequencing</t>
+        </is>
+      </c>
+      <c r="AY5" s="2" t="inlineStr">
+        <is>
+          <t>other</t>
+        </is>
+      </c>
+      <c r="AZ5" s="2" t="inlineStr">
+        <is>
+          <t>other</t>
+        </is>
+      </c>
+      <c r="BA5" s="2" t="inlineStr">
+        <is>
+          <t>other</t>
+        </is>
+      </c>
+      <c r="BB5" s="2" t="inlineStr">
+        <is>
+          <t>other</t>
+        </is>
+      </c>
+      <c r="BC5" s="2" t="inlineStr">
+        <is>
+          <t>other</t>
+        </is>
+      </c>
+      <c r="BD5" s="2" t="inlineStr">
+        <is>
+          <t>other</t>
+        </is>
+      </c>
+      <c r="BE5" s="2" t="inlineStr">
+        <is>
+          <t>other</t>
+        </is>
+      </c>
+      <c r="BF5" s="2" t="inlineStr">
+        <is>
+          <t>other</t>
+        </is>
+      </c>
+      <c r="BG5" s="2" t="inlineStr">
+        <is>
+          <t>other</t>
+        </is>
+      </c>
+      <c r="BH5" s="2" t="inlineStr">
+        <is>
+          <t>other</t>
+        </is>
+      </c>
+      <c r="BI5" s="2" t="inlineStr">
+        <is>
+          <t>other</t>
+        </is>
+      </c>
+      <c r="BJ5" s="2" t="inlineStr">
+        <is>
+          <t>other</t>
+        </is>
+      </c>
     </row>
     <row r="6" ht="25" customHeight="1">
       <c r="A6" s="2" t="inlineStr">
         <is>
-          <t>category</t>
+          <t>regex</t>
         </is>
       </c>
       <c r="B6" s="2" t="inlineStr"/>
-      <c r="C6" s="2" t="inlineStr">
-        <is>
-          <t>sample</t>
-        </is>
-      </c>
-      <c r="D6" s="2" t="inlineStr">
-        <is>
-          <t>sample</t>
-        </is>
-      </c>
-      <c r="E6" s="2" t="inlineStr">
-        <is>
-          <t>sample</t>
-        </is>
-      </c>
-      <c r="F6" s="2" t="inlineStr">
-        <is>
-          <t>sample</t>
-        </is>
-      </c>
-      <c r="G6" s="2" t="inlineStr">
-        <is>
-          <t>sample</t>
-        </is>
-      </c>
-      <c r="H6" s="2" t="inlineStr">
-        <is>
-          <t>sample</t>
-        </is>
-      </c>
-      <c r="I6" s="2" t="inlineStr">
-        <is>
-          <t>sample</t>
-        </is>
-      </c>
-      <c r="J6" s="2" t="inlineStr">
-        <is>
-          <t>sample</t>
-        </is>
-      </c>
-      <c r="K6" s="2" t="inlineStr">
-        <is>
-          <t>sample</t>
-        </is>
-      </c>
-      <c r="L6" s="2" t="inlineStr">
-        <is>
-          <t>sample</t>
-        </is>
-      </c>
-      <c r="M6" s="2" t="inlineStr">
-        <is>
-          <t>sample</t>
-        </is>
-      </c>
-      <c r="N6" s="2" t="inlineStr">
-        <is>
-          <t>sample</t>
-        </is>
-      </c>
-      <c r="O6" s="2" t="inlineStr">
-        <is>
-          <t>sample</t>
-        </is>
-      </c>
-      <c r="P6" s="2" t="inlineStr">
-        <is>
-          <t>sample</t>
-        </is>
-      </c>
-      <c r="Q6" s="2" t="inlineStr">
-        <is>
-          <t>sample</t>
-        </is>
-      </c>
-      <c r="R6" s="2" t="inlineStr">
-        <is>
-          <t>sample</t>
-        </is>
-      </c>
-      <c r="S6" s="2" t="inlineStr">
-        <is>
-          <t>experiment</t>
-        </is>
-      </c>
-      <c r="T6" s="2" t="inlineStr">
-        <is>
-          <t>experiment</t>
-        </is>
-      </c>
-      <c r="U6" s="2" t="inlineStr">
-        <is>
-          <t>experiment</t>
-        </is>
-      </c>
-      <c r="V6" s="2" t="inlineStr">
-        <is>
-          <t>experiment</t>
-        </is>
-      </c>
-      <c r="W6" s="2" t="inlineStr">
-        <is>
-          <t>experiment</t>
-        </is>
-      </c>
-      <c r="X6" s="2" t="inlineStr">
-        <is>
-          <t>experiment</t>
-        </is>
-      </c>
-      <c r="Y6" s="2" t="inlineStr">
-        <is>
-          <t>experiment</t>
-        </is>
-      </c>
+      <c r="C6" s="2" t="inlineStr"/>
+      <c r="D6" s="2" t="inlineStr"/>
+      <c r="E6" s="2" t="inlineStr"/>
+      <c r="F6" s="2" t="inlineStr"/>
+      <c r="G6" s="2" t="inlineStr"/>
+      <c r="H6" s="2" t="inlineStr"/>
+      <c r="I6" s="2" t="inlineStr"/>
+      <c r="J6" s="2" t="inlineStr"/>
+      <c r="K6" s="2" t="inlineStr"/>
+      <c r="L6" s="2" t="inlineStr"/>
+      <c r="M6" s="2" t="inlineStr"/>
+      <c r="N6" s="2" t="inlineStr"/>
+      <c r="O6" s="2" t="inlineStr"/>
+      <c r="P6" s="2" t="inlineStr"/>
+      <c r="Q6" s="2" t="inlineStr"/>
+      <c r="R6" s="2" t="inlineStr"/>
+      <c r="S6" s="2" t="inlineStr"/>
+      <c r="T6" s="2" t="inlineStr"/>
+      <c r="U6" s="2" t="inlineStr"/>
+      <c r="V6" s="2" t="inlineStr"/>
+      <c r="W6" s="2" t="inlineStr"/>
+      <c r="X6" s="2" t="inlineStr"/>
+      <c r="Y6" s="2" t="inlineStr"/>
       <c r="Z6" s="2" t="inlineStr">
         <is>
-          <t>experiment</t>
+          <t>[+-]?([0-9]*[.])?[0-9]+</t>
         </is>
       </c>
       <c r="AA6" s="2" t="inlineStr">
         <is>
-          <t>experiment</t>
+          <t>[+-]?([0-9]*[.])?[0-9]+</t>
         </is>
       </c>
       <c r="AB6" s="2" t="inlineStr">
         <is>
-          <t>experiment</t>
+          <t>[0-9]*</t>
         </is>
       </c>
       <c r="AC6" s="2" t="inlineStr">
         <is>
-          <t>experiment</t>
+          <t>[0-9]*</t>
         </is>
       </c>
       <c r="AD6" s="2" t="inlineStr">
         <is>
-          <t>experiment</t>
+          <t>[+-]?([0-9]*[.])?[0-9]+</t>
         </is>
       </c>
       <c r="AE6" s="2" t="inlineStr">
         <is>
-          <t>experiment</t>
+          <t>[0-9]*</t>
         </is>
       </c>
       <c r="AF6" s="2" t="inlineStr">
         <is>
-          <t>experiment</t>
-        </is>
-      </c>
-      <c r="AG6" s="2" t="inlineStr">
-        <is>
-          <t>experiment</t>
-        </is>
-      </c>
-      <c r="AH6" s="2" t="inlineStr">
-        <is>
-          <t>experiment</t>
-        </is>
-      </c>
+          <t>[+-]?([0-9]*[.])?[0-9]+</t>
+        </is>
+      </c>
+      <c r="AG6" s="2" t="inlineStr"/>
+      <c r="AH6" s="2" t="inlineStr"/>
       <c r="AI6" s="2" t="inlineStr">
         <is>
-          <t>experiment</t>
-        </is>
-      </c>
-      <c r="AJ6" s="2" t="inlineStr">
-        <is>
-          <t>experiment</t>
-        </is>
-      </c>
+          <t>[ATGC]*</t>
+        </is>
+      </c>
+      <c r="AJ6" s="2" t="inlineStr"/>
       <c r="AK6" s="2" t="inlineStr">
         <is>
-          <t>experiment</t>
-        </is>
-      </c>
-      <c r="AL6" s="2" t="inlineStr">
-        <is>
-          <t>experiment</t>
-        </is>
-      </c>
-      <c r="AM6" s="2" t="inlineStr">
-        <is>
-          <t>experiment</t>
-        </is>
-      </c>
-      <c r="AN6" s="2" t="inlineStr">
-        <is>
-          <t>sequencing</t>
-        </is>
-      </c>
+          <t>[ATGC, ]*</t>
+        </is>
+      </c>
+      <c r="AL6" s="2" t="inlineStr"/>
+      <c r="AM6" s="2" t="inlineStr"/>
+      <c r="AN6" s="2" t="inlineStr"/>
       <c r="AO6" s="2" t="inlineStr">
         <is>
-          <t>sequencing</t>
+          <t>[0-9]*</t>
         </is>
       </c>
       <c r="AP6" s="2" t="inlineStr">
         <is>
-          <t>sequencing</t>
+          <t>[A-Z]{2}[0-9]{4}[0-9]{2}[0-9]{2}</t>
         </is>
       </c>
       <c r="AQ6" s="2" t="inlineStr">
         <is>
-          <t>sequencing</t>
+          <t>[0-9]*</t>
         </is>
       </c>
       <c r="AR6" s="2" t="inlineStr">
         <is>
-          <t>sequencing</t>
-        </is>
-      </c>
-      <c r="AS6" s="2" t="inlineStr">
-        <is>
-          <t>sequencing</t>
-        </is>
-      </c>
-      <c r="AT6" s="2" t="inlineStr">
-        <is>
-          <t>sequencing</t>
-        </is>
-      </c>
-      <c r="AU6" s="2" t="inlineStr">
-        <is>
-          <t>sequencing</t>
-        </is>
-      </c>
+          <t>[0-9]{5,}</t>
+        </is>
+      </c>
+      <c r="AS6" s="2" t="inlineStr"/>
+      <c r="AT6" s="2" t="inlineStr"/>
+      <c r="AU6" s="2" t="inlineStr"/>
       <c r="AV6" s="2" t="inlineStr">
         <is>
-          <t>sequencing</t>
+          <t>[0-9]{1,2}</t>
         </is>
       </c>
       <c r="AW6" s="2" t="inlineStr">
         <is>
-          <t>sequencing</t>
+          <t>[A-Z]</t>
         </is>
       </c>
       <c r="AX6" s="2" t="inlineStr">
         <is>
-          <t>sequencing</t>
-        </is>
-      </c>
-      <c r="AY6" s="2" t="inlineStr">
-        <is>
-          <t>other</t>
-        </is>
-      </c>
-      <c r="AZ6" s="2" t="inlineStr">
-        <is>
-          <t>other</t>
-        </is>
-      </c>
-      <c r="BA6" s="2" t="inlineStr">
-        <is>
-          <t>other</t>
-        </is>
-      </c>
-      <c r="BB6" s="2" t="inlineStr">
-        <is>
-          <t>other</t>
-        </is>
-      </c>
-      <c r="BC6" s="2" t="inlineStr">
-        <is>
-          <t>other</t>
-        </is>
-      </c>
-      <c r="BD6" s="2" t="inlineStr">
-        <is>
-          <t>other</t>
-        </is>
-      </c>
-      <c r="BE6" s="2" t="inlineStr">
-        <is>
-          <t>other</t>
-        </is>
-      </c>
-      <c r="BF6" s="2" t="inlineStr">
-        <is>
-          <t>other</t>
-        </is>
-      </c>
-      <c r="BG6" s="2" t="inlineStr">
-        <is>
-          <t>other</t>
-        </is>
-      </c>
-      <c r="BH6" s="2" t="inlineStr">
-        <is>
-          <t>other</t>
-        </is>
-      </c>
-      <c r="BI6" s="2" t="inlineStr">
-        <is>
-          <t>other</t>
-        </is>
-      </c>
-      <c r="BJ6" s="2" t="inlineStr">
-        <is>
-          <t>other</t>
-        </is>
-      </c>
-    </row>
-    <row r="7" ht="25" customHeight="1">
-      <c r="A7" s="2" t="inlineStr">
-        <is>
-          <t>regex</t>
-        </is>
-      </c>
-      <c r="B7" s="2" t="inlineStr"/>
-      <c r="C7" s="2" t="inlineStr"/>
-      <c r="D7" s="2" t="inlineStr"/>
-      <c r="E7" s="2" t="inlineStr"/>
-      <c r="F7" s="2" t="inlineStr"/>
-      <c r="G7" s="2" t="inlineStr"/>
-      <c r="H7" s="2" t="inlineStr"/>
-      <c r="I7" s="2" t="inlineStr"/>
-      <c r="J7" s="2" t="inlineStr"/>
-      <c r="K7" s="2" t="inlineStr"/>
-      <c r="L7" s="2" t="inlineStr"/>
-      <c r="M7" s="2" t="inlineStr"/>
-      <c r="N7" s="2" t="inlineStr"/>
-      <c r="O7" s="2" t="inlineStr"/>
-      <c r="P7" s="2" t="inlineStr"/>
-      <c r="Q7" s="2" t="inlineStr"/>
-      <c r="R7" s="2" t="inlineStr"/>
-      <c r="S7" s="2" t="inlineStr"/>
-      <c r="T7" s="2" t="inlineStr"/>
-      <c r="U7" s="2" t="inlineStr"/>
-      <c r="V7" s="2" t="inlineStr"/>
-      <c r="W7" s="2" t="inlineStr"/>
-      <c r="X7" s="2" t="inlineStr"/>
-      <c r="Y7" s="2" t="inlineStr"/>
-      <c r="Z7" s="2" t="inlineStr">
-        <is>
-          <t>[+-]?([0-9]*[.])?[0-9]+</t>
-        </is>
-      </c>
-      <c r="AA7" s="2" t="inlineStr">
-        <is>
-          <t>[+-]?([0-9]*[.])?[0-9]+</t>
-        </is>
-      </c>
-      <c r="AB7" s="2" t="inlineStr">
-        <is>
-          <t>[0-9]*</t>
-        </is>
-      </c>
-      <c r="AC7" s="2" t="inlineStr">
-        <is>
-          <t>[0-9]*</t>
-        </is>
-      </c>
-      <c r="AD7" s="2" t="inlineStr">
-        <is>
-          <t>[+-]?([0-9]*[.])?[0-9]+</t>
-        </is>
-      </c>
-      <c r="AE7" s="2" t="inlineStr">
-        <is>
-          <t>[0-9]*</t>
-        </is>
-      </c>
-      <c r="AF7" s="2" t="inlineStr">
-        <is>
-          <t>[+-]?([0-9]*[.])?[0-9]+</t>
-        </is>
-      </c>
-      <c r="AG7" s="2" t="inlineStr"/>
-      <c r="AH7" s="2" t="inlineStr"/>
-      <c r="AI7" s="2" t="inlineStr">
-        <is>
-          <t>[ATGC]*</t>
-        </is>
-      </c>
-      <c r="AJ7" s="2" t="inlineStr"/>
-      <c r="AK7" s="2" t="inlineStr">
-        <is>
-          <t>[ATGC, ]*</t>
-        </is>
-      </c>
-      <c r="AL7" s="2" t="inlineStr"/>
-      <c r="AM7" s="2" t="inlineStr"/>
-      <c r="AN7" s="2" t="inlineStr"/>
-      <c r="AO7" s="2" t="inlineStr">
-        <is>
-          <t>[0-9]*</t>
-        </is>
-      </c>
-      <c r="AP7" s="2" t="inlineStr">
-        <is>
-          <t>[A-Z]{2}[0-9]{4}[0-9]{2}[0-9]{2}</t>
-        </is>
-      </c>
-      <c r="AQ7" s="2" t="inlineStr">
-        <is>
-          <t>[0-9]*</t>
-        </is>
-      </c>
-      <c r="AR7" s="2" t="inlineStr">
-        <is>
-          <t>[0-9]{5,}</t>
-        </is>
-      </c>
-      <c r="AS7" s="2" t="inlineStr"/>
-      <c r="AT7" s="2" t="inlineStr"/>
-      <c r="AU7" s="2" t="inlineStr"/>
-      <c r="AV7" s="2" t="inlineStr">
-        <is>
-          <t>[0-9]{1,2}</t>
-        </is>
-      </c>
-      <c r="AW7" s="2" t="inlineStr">
-        <is>
-          <t>[A-Z]</t>
-        </is>
-      </c>
-      <c r="AX7" s="2" t="inlineStr">
-        <is>
           <t>[0-9]{1,2}[A-Z]</t>
         </is>
       </c>
-      <c r="AY7" s="2" t="inlineStr"/>
-      <c r="AZ7" s="2" t="inlineStr"/>
-      <c r="BA7" s="2" t="inlineStr"/>
-      <c r="BB7" s="2" t="inlineStr"/>
-      <c r="BC7" s="2" t="inlineStr"/>
-      <c r="BD7" s="2" t="inlineStr"/>
-      <c r="BE7" s="2" t="inlineStr"/>
-      <c r="BF7" s="2" t="inlineStr"/>
-      <c r="BG7" s="2" t="inlineStr"/>
-      <c r="BH7" s="2" t="inlineStr"/>
-      <c r="BI7" s="2" t="inlineStr"/>
-      <c r="BJ7" s="2" t="inlineStr"/>
+      <c r="AY6" s="2" t="inlineStr"/>
+      <c r="AZ6" s="2" t="inlineStr"/>
+      <c r="BA6" s="2" t="inlineStr"/>
+      <c r="BB6" s="2" t="inlineStr"/>
+      <c r="BC6" s="2" t="inlineStr"/>
+      <c r="BD6" s="2" t="inlineStr"/>
+      <c r="BE6" s="2" t="inlineStr"/>
+      <c r="BF6" s="2" t="inlineStr"/>
+      <c r="BG6" s="2" t="inlineStr"/>
+      <c r="BH6" s="2" t="inlineStr"/>
+      <c r="BI6" s="2" t="inlineStr"/>
+      <c r="BJ6" s="2" t="inlineStr"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>